<commit_message>
Forgot to add case-design files
files were created a long time ago. Just forgot to add them into the repo
</commit_message>
<xml_diff>
--- a/Bill-Of-Material/BOM_PCB_Project.xlsx
+++ b/Bill-Of-Material/BOM_PCB_Project.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oliwi\Desktop\Project_Ontwerpen_1stejaar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oliwi\Desktop\elektor_wekker\Project_Ontwerpen_1stejaar\Bill-Of-Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD969D8-B5FA-47F6-AF8A-DDA1D1E50F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DA49CD-0CAD-47DE-85BF-4DD9521D4ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C2354DA8-8B92-41B3-A2F9-7477D9FACADF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C2354DA8-8B92-41B3-A2F9-7477D9FACADF}"/>
   </bookViews>
   <sheets>
     <sheet name="PCB_Project" sheetId="1" r:id="rId1"/>
@@ -503,12 +503,6 @@
     <t>case voor project</t>
   </si>
   <si>
-    <t>sponsor: Thibe VanOrshaegen</t>
-  </si>
-  <si>
-    <t>Totaal:</t>
-  </si>
-  <si>
     <t>Vishay / Dale</t>
   </si>
   <si>
@@ -600,14 +594,21 @@
   </si>
   <si>
     <t>Verzendkosten</t>
+  </si>
+  <si>
+    <t>Totaal(euro):</t>
+  </si>
+  <si>
+    <t>Thibe VanOrshaegen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -657,7 +658,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -704,23 +705,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -728,13 +718,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1073,23 +1061,23 @@
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="63" workbookViewId="0">
-      <selection activeCell="N37" sqref="N37"/>
+      <selection activeCell="M54" sqref="M54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
     <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" customWidth="1"/>
-    <col min="9" max="9" width="21.77734375" customWidth="1"/>
-    <col min="10" max="10" width="19.33203125" customWidth="1"/>
-    <col min="11" max="11" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1124,7 +1112,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -1155,12 +1143,12 @@
       <c r="J2" s="1">
         <v>13.28</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2" s="10">
         <f>J2*E2</f>
         <v>13.28</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -1191,12 +1179,12 @@
       <c r="J3" s="1">
         <v>0.34399999999999997</v>
       </c>
-      <c r="K3" s="1">
-        <f t="shared" ref="K3:K42" si="0">J3*E3</f>
+      <c r="K3" s="10">
+        <f t="shared" ref="K3:K40" si="0">J3*E3</f>
         <v>0.34399999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -1227,12 +1215,12 @@
       <c r="J4" s="1">
         <v>0.307</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="10">
         <f t="shared" si="0"/>
         <v>0.61399999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -1249,26 +1237,26 @@
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>158</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>114</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J5" s="1">
         <v>0.22</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="10">
         <f t="shared" si="0"/>
         <v>0.22</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1285,26 +1273,26 @@
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>114</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J6" s="1">
         <v>0.52100000000000002</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="10">
         <f t="shared" si="0"/>
         <v>0.52100000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1321,26 +1309,26 @@
         <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>114</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J7" s="1">
         <v>0.90200000000000002</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="10">
         <f t="shared" si="0"/>
         <v>6.3140000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1357,26 +1345,26 @@
         <v>3</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>114</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="J8" s="1">
         <v>0.52100000000000002</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="10">
         <f t="shared" si="0"/>
         <v>1.5630000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -1393,26 +1381,26 @@
         <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>114</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J9" s="1">
         <v>0.20499999999999999</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="10">
         <f t="shared" si="0"/>
         <v>0.20499999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -1429,26 +1417,26 @@
         <v>3</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>114</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J10" s="1">
         <v>0.158</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="10">
         <f t="shared" si="0"/>
         <v>0.47399999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1465,26 +1453,26 @@
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>114</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J11" s="1">
         <v>0.51200000000000001</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11" s="10">
         <f t="shared" si="0"/>
         <v>0.51200000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -1501,26 +1489,26 @@
         <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>114</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J12" s="1">
         <v>0.90200000000000002</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="10">
         <f t="shared" si="0"/>
         <v>0.90200000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -1551,12 +1539,12 @@
       <c r="J13" s="1">
         <v>10.5</v>
       </c>
-      <c r="K13" s="1">
+      <c r="K13" s="10">
         <f t="shared" si="0"/>
         <v>10.5</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -1587,12 +1575,12 @@
       <c r="J14" s="1">
         <v>2.14</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K14" s="10">
         <f t="shared" si="0"/>
         <v>17.12</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
@@ -1623,12 +1611,12 @@
       <c r="J15" s="1">
         <v>0.372</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15" s="10">
         <f t="shared" si="0"/>
         <v>0.372</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
@@ -1659,12 +1647,12 @@
       <c r="J16" s="1">
         <v>0.49</v>
       </c>
-      <c r="K16" s="1">
+      <c r="K16" s="10">
         <f t="shared" si="0"/>
         <v>0.98</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>11</v>
       </c>
@@ -1695,12 +1683,12 @@
       <c r="J17" s="1">
         <v>0.74</v>
       </c>
-      <c r="K17" s="1">
+      <c r="K17" s="10">
         <f t="shared" si="0"/>
         <v>0.74</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
@@ -1731,12 +1719,12 @@
       <c r="J18" s="1">
         <v>0.49</v>
       </c>
-      <c r="K18" s="1">
+      <c r="K18" s="10">
         <f t="shared" si="0"/>
         <v>0.98</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>11</v>
       </c>
@@ -1767,12 +1755,12 @@
       <c r="J19" s="1">
         <v>0.42</v>
       </c>
-      <c r="K19" s="1">
+      <c r="K19" s="10">
         <f t="shared" si="0"/>
         <v>0.84</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>11</v>
       </c>
@@ -1803,12 +1791,12 @@
       <c r="J20" s="1">
         <v>0.38100000000000001</v>
       </c>
-      <c r="K20" s="1">
+      <c r="K20" s="10">
         <f t="shared" si="0"/>
         <v>0.38100000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>11</v>
       </c>
@@ -1839,12 +1827,12 @@
       <c r="J21" s="1">
         <v>10.93</v>
       </c>
-      <c r="K21" s="1">
+      <c r="K21" s="10">
         <f t="shared" si="0"/>
         <v>10.93</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
@@ -1875,12 +1863,12 @@
       <c r="J22" s="1">
         <v>1.17</v>
       </c>
-      <c r="K22" s="1">
+      <c r="K22" s="10">
         <f t="shared" si="0"/>
         <v>1.17</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>11</v>
       </c>
@@ -1911,12 +1899,12 @@
       <c r="J23" s="1">
         <v>0.995</v>
       </c>
-      <c r="K23" s="1">
+      <c r="K23" s="10">
         <f t="shared" si="0"/>
         <v>0.995</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
@@ -1947,12 +1935,12 @@
       <c r="J24" s="1">
         <v>12.41</v>
       </c>
-      <c r="K24" s="1">
+      <c r="K24" s="10">
         <f t="shared" si="0"/>
         <v>12.41</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
@@ -1983,12 +1971,12 @@
       <c r="J25" s="1">
         <v>0.74</v>
       </c>
-      <c r="K25" s="1">
+      <c r="K25" s="10">
         <f t="shared" si="0"/>
         <v>0.74</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>11</v>
       </c>
@@ -2019,12 +2007,12 @@
       <c r="J26" s="1">
         <v>0.17699999999999999</v>
       </c>
-      <c r="K26" s="1">
+      <c r="K26" s="10">
         <f t="shared" si="0"/>
         <v>0.70799999999999996</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>11</v>
       </c>
@@ -2055,12 +2043,12 @@
       <c r="J27" s="1">
         <v>0.93</v>
       </c>
-      <c r="K27" s="1">
+      <c r="K27" s="10">
         <f t="shared" si="0"/>
         <v>0.93</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>11</v>
       </c>
@@ -2091,12 +2079,12 @@
       <c r="J28" s="1">
         <v>0.33500000000000002</v>
       </c>
-      <c r="K28" s="1">
+      <c r="K28" s="10">
         <f t="shared" si="0"/>
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>11</v>
       </c>
@@ -2127,12 +2115,12 @@
       <c r="J29" s="1">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="K29" s="1">
+      <c r="K29" s="10">
         <f t="shared" si="0"/>
         <v>0.372</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>11</v>
       </c>
@@ -2149,10 +2137,10 @@
         <v>1</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>106</v>
@@ -2163,12 +2151,12 @@
       <c r="J30" s="1">
         <v>0.01</v>
       </c>
-      <c r="K30" s="1">
+      <c r="K30" s="10">
         <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
         <v>84</v>
@@ -2183,10 +2171,10 @@
         <v>1</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>106</v>
@@ -2197,12 +2185,12 @@
       <c r="J31" s="1">
         <v>1.49</v>
       </c>
-      <c r="K31" s="1">
+      <c r="K31" s="10">
         <f t="shared" si="0"/>
         <v>1.49</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>11</v>
       </c>
@@ -2219,10 +2207,10 @@
         <v>3</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>106</v>
@@ -2233,12 +2221,12 @@
       <c r="J32" s="1">
         <v>0.03</v>
       </c>
-      <c r="K32" s="1">
+      <c r="K32" s="10">
         <f t="shared" si="0"/>
         <v>0.09</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
         <v>89</v>
@@ -2253,10 +2241,10 @@
         <v>1</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>106</v>
@@ -2267,12 +2255,12 @@
       <c r="J33" s="1">
         <v>1.03</v>
       </c>
-      <c r="K33" s="1">
+      <c r="K33" s="10">
         <f t="shared" si="0"/>
         <v>1.03</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
         <v>91</v>
@@ -2287,10 +2275,10 @@
         <v>1</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>106</v>
@@ -2301,12 +2289,12 @@
       <c r="J34" s="1">
         <v>0.14000000000000001</v>
       </c>
-      <c r="K34" s="1">
+      <c r="K34" s="10">
         <f t="shared" si="0"/>
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>11</v>
       </c>
@@ -2326,7 +2314,7 @@
         <v>123</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>106</v>
@@ -2337,12 +2325,12 @@
       <c r="J35" s="1">
         <v>0.05</v>
       </c>
-      <c r="K35" s="1">
+      <c r="K35" s="10">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
         <v>95</v>
@@ -2357,10 +2345,10 @@
         <v>1</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>106</v>
@@ -2371,12 +2359,12 @@
       <c r="J36" s="1">
         <v>0.21</v>
       </c>
-      <c r="K36" s="1">
+      <c r="K36" s="10">
         <f t="shared" si="0"/>
         <v>0.21</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
         <v>97</v>
@@ -2391,26 +2379,26 @@
         <v>1</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>124</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="J37" s="1">
         <v>0.23</v>
       </c>
-      <c r="K37" s="1">
+      <c r="K37" s="10">
         <f t="shared" si="0"/>
         <v>0.23</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
         <v>99</v>
@@ -2425,10 +2413,10 @@
         <v>1</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>106</v>
@@ -2439,12 +2427,12 @@
       <c r="J38" s="1">
         <v>0.25</v>
       </c>
-      <c r="K38" s="1">
+      <c r="K38" s="10">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>11</v>
       </c>
@@ -2475,12 +2463,12 @@
       <c r="J39" s="1">
         <v>0.64200000000000002</v>
       </c>
-      <c r="K39" s="1">
+      <c r="K39" s="10">
         <f t="shared" si="0"/>
         <v>0.64200000000000002</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>11</v>
       </c>
@@ -2511,15 +2499,15 @@
       <c r="J40" s="1">
         <v>1.54</v>
       </c>
-      <c r="K40" s="1">
+      <c r="K40" s="10">
         <f t="shared" si="0"/>
         <v>1.54</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A41" s="13"/>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="9"/>
       <c r="B41" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>151</v>
@@ -2545,12 +2533,12 @@
       <c r="J41" s="1">
         <v>7.5</v>
       </c>
-      <c r="K41" s="1">
+      <c r="K41" s="10">
         <f>J41</f>
         <v>7.5</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -2561,19 +2549,16 @@
       <c r="H42" s="6"/>
       <c r="I42" s="6"/>
       <c r="J42" s="6"/>
-      <c r="K42" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K42" s="11"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>148</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" t="s">
         <v>149</v>
       </c>
-      <c r="E43" s="7">
+      <c r="E43">
         <v>5</v>
       </c>
       <c r="F43" t="s">
@@ -2588,7 +2573,7 @@
       <c r="I43" t="s">
         <v>151</v>
       </c>
-      <c r="J43" s="12">
+      <c r="J43" s="1">
         <v>69.989999999999995</v>
       </c>
       <c r="K43" s="10">
@@ -2596,18 +2581,18 @@
         <v>69.989999999999995</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>152</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" t="s">
         <v>153</v>
       </c>
-      <c r="E44" s="7">
+      <c r="E44">
         <v>1</v>
       </c>
       <c r="F44" t="s">
-        <v>154</v>
+        <v>186</v>
       </c>
       <c r="G44" t="s">
         <v>151</v>
@@ -2618,30 +2603,30 @@
       <c r="I44" t="s">
         <v>151</v>
       </c>
-      <c r="J44" s="12">
-        <v>0</v>
-      </c>
-      <c r="K44" s="11">
+      <c r="J44" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="K44" s="10">
         <f>J44</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A45" s="8"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
-      <c r="I45" s="8"/>
-      <c r="J45" s="9" t="s">
-        <v>155</v>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="7"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="8" t="s">
+        <v>185</v>
       </c>
       <c r="K45" s="10">
         <f>SUM(K2:K44)</f>
-        <v>168.67399999999998</v>
+        <v>171.17399999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>